<commit_message>
plots of warning type and snippet distribution for each tool
</commit_message>
<xml_diff>
--- a/meta-analysis/correlation_analysis_for_meta_analysis.xlsx
+++ b/meta-analysis/correlation_analysis_for_meta_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ojcchar/repositories/Projects/complexity-verification-project/meta-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F55F3D0-2966-A54E-A81C-892BF17B154F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19F0A82-8426-ED41-8C6E-E95C3D746627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_tools" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,19 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">infer!$A$1:$L$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">typestate_checker!$A$1:$L$19</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -540,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView zoomScale="143" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1296,8 +1308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2005,7 +2017,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2713,7 +2725,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="G11" activeCellId="1" sqref="G16 G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>